<commit_message>
Carina's xlsx and my conversion of it to TTL
</commit_message>
<xml_diff>
--- a/ec-m4m-variables.xlsx
+++ b/ec-m4m-variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgraybeal/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/carinaj/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B1E942-C4F9-4F48-B65A-93A798371E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F2A8DFE-25A4-C840-88FA-89F1971F49D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48360" yWindow="5520" windowWidth="31560" windowHeight="17840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-320" yWindow="500" windowWidth="50240" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="controlled-terminology" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="128">
   <si>
     <t>ConceptScheme URI</t>
   </si>
@@ -459,9 +459,6 @@
     <t>Identifier if poss.</t>
   </si>
   <si>
-    <t xml:space="preserve">https://orcid.org/0000-0001-6875-5360 </t>
-  </si>
-  <si>
     <t>https://purl.org/ecm4m/vocs</t>
   </si>
   <si>
@@ -567,10 +564,52 @@
     <t>ecm4m-voc:Non-PolishedSectionContainerType</t>
   </si>
   <si>
-    <t>ecm4m-voc:PolishedSectionsampletype</t>
-  </si>
-  <si>
     <t>ecm4m-voc:PolishedSectionContainerType</t>
+  </si>
+  <si>
+    <t>ecm4m-voc:PolishedSectionSampletype</t>
+  </si>
+  <si>
+    <t>https://orcid.org/0000-0002-0972-6321</t>
+  </si>
+  <si>
+    <t>Residues are solids leftover after dissolution of samples and subsequent chemical processing.</t>
+  </si>
+  <si>
+    <t>FIB sections are milled out of samples with a focused ion beam (FIB).</t>
+  </si>
+  <si>
+    <t>Atom probe tips are needle-shaped samples milled out of samples with a focused ion beam (FIB).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microtome slices are prepared by cutting a particle embedded in an epoxy bullet into numerous slices with a ultramicrotome. Multiple slices will be deposited onto a single TEM grid. When this happens the grid will be given a single sample name, not the individual slices within it. </t>
+  </si>
+  <si>
+    <t>Solution that a solid sample has been extracted into.</t>
+  </si>
+  <si>
+    <t>Aggregate samples are collections of particles; the particles in aggregate samples have not been intentionally modified. The particles in aggregate samples do not necessarily have any relationship to each other aside from being returned OSIRIS-REx material.</t>
+  </si>
+  <si>
+    <t>Powders are samples that have been intentionally modified to reduce the average particle size. Powders can be generated by pulverizing particles, chips, and/or aggregate samples.</t>
+  </si>
+  <si>
+    <t>A chip is a piece intentionally broken off a particle or a piece that is observed and documented to have broken off a particle.</t>
+  </si>
+  <si>
+    <t>A particle is a competent individual geologic sample of any size.</t>
+  </si>
+  <si>
+    <t>Samples mounted onto a glass slide and polished to a thickness of ~30 µm. Thin sections made at JSC are polished on both sides (the side adhered to the glass with epoxy and the exposed side).</t>
+  </si>
+  <si>
+    <t>Samples may be polished on only one side. The sample thickness is greater than a standard thin section (~30 µm) – the desired thickness should be specified. Thick sections are typically mounted onto a glass slide when prepared at JSC thick sections on a glass slide are polished on both sides.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Potted butts are sample pieces mounted in epoxy from which multiple thin or thick sections can be made. In the event that it is not possible to make a thin or thick section of any particle, potted butts may be the primary sample preparation and holder for in situ analyses. </t>
+  </si>
+  <si>
+    <t>Grain mounts typically include multiple pieces of sample mounted (in epoxy or metal) and polished on one exposed side.</t>
   </si>
 </sst>
 </file>
@@ -902,21 +941,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="61">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -934,45 +973,45 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -982,19 +1021,23 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1002,9 +1045,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1016,7 +1056,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1249,10 +1288,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C27" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="E52" sqref="E52:E57"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
@@ -1280,7 +1319,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>28</v>
@@ -1304,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C3" s="13" t="str">
         <f>B1 &amp; "/"</f>
@@ -1371,11 +1410,11 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="31" customHeight="1">
-      <c r="A8" s="56" t="s">
+      <c r="A8" s="54" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="56"/>
-      <c r="C8" s="56"/>
+      <c r="B8" s="54"/>
+      <c r="C8" s="54"/>
       <c r="D8" s="34"/>
     </row>
     <row r="9" spans="1:4" ht="16">
@@ -1383,7 +1422,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>35</v>
@@ -1394,7 +1433,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>44</v>
@@ -1405,7 +1444,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>45</v>
@@ -1416,7 +1455,7 @@
         <v>36</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="16"/>
       <c r="D12" s="35" t="s">
@@ -1428,7 +1467,7 @@
         <v>7</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>77</v>
+        <v>114</v>
       </c>
       <c r="D13" s="35" t="s">
         <v>49</v>
@@ -1451,7 +1490,7 @@
         <v>40</v>
       </c>
       <c r="B15" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D15" s="35" t="s">
         <v>50</v>
@@ -1474,18 +1513,18 @@
       </c>
       <c r="B17" s="18" t="str">
         <f ca="1">TEXT(NOW(),"yyyy-mm-ddThh:MM:ss") &amp; "-07:00"</f>
-        <v>2022-09-07T21:32:11-07:00</v>
+        <v>2022-09-08T11:15:14-07:00</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:17" ht="31" customHeight="1">
-      <c r="A18" s="56" t="s">
+      <c r="A18" s="54" t="s">
         <v>55</v>
       </c>
-      <c r="B18" s="56"/>
-      <c r="C18" s="56"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:17" ht="16">
@@ -1534,29 +1573,29 @@
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:17" ht="34" customHeight="1">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
-      <c r="D25" s="59"/>
-      <c r="E25" s="53" t="s">
+      <c r="B25" s="59"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="F25" s="54"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="54"/>
-      <c r="I25" s="55"/>
-      <c r="J25" s="53" t="s">
+      <c r="F25" s="56"/>
+      <c r="G25" s="56"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="K25" s="54"/>
-      <c r="L25" s="54"/>
-      <c r="M25" s="54"/>
-      <c r="N25" s="54"/>
-      <c r="O25" s="54"/>
-      <c r="P25" s="55"/>
-      <c r="Q25" s="60"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="P25" s="57"/>
+      <c r="Q25" s="53"/>
     </row>
     <row r="26" spans="1:17" s="36" customFormat="1" ht="36" customHeight="1">
       <c r="A26" s="11"/>
@@ -1659,10 +1698,10 @@
         <v>ecm4m-voc:Non-PolishedSectionSampleType</v>
       </c>
       <c r="B28" s="25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D28" s="25"/>
       <c r="E28" s="27"/>
@@ -1686,12 +1725,14 @@
         <v>ecm4m-voc:powder</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C29" s="4"/>
+        <v>109</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>121</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F29" s="31"/>
       <c r="G29" s="31"/>
@@ -1711,12 +1752,14 @@
         <v>ecm4m-voc:aggregate</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C30" s="3"/>
+        <v>97</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>120</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
@@ -1736,12 +1779,14 @@
         <v>ecm4m-voc:chip</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="C31" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>122</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F31" s="31"/>
       <c r="G31" s="31"/>
@@ -1757,16 +1802,18 @@
     </row>
     <row r="32" spans="1:17" ht="15" customHeight="1">
       <c r="A32" s="23" t="str">
-        <f t="shared" ref="A32:A63" si="2">IF(ISBLANK($B32),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B32," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A32:A62" si="2">IF(ISBLANK($B32),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B32," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ecm4m-voc:particle</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>123</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
@@ -1786,12 +1833,14 @@
         <v>ecm4m-voc:liquid</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C33" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>119</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F33" s="31"/>
       <c r="G33" s="31"/>
@@ -1811,12 +1860,14 @@
         <v>ecm4m-voc:fibsection</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="C34" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>116</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="30"/>
@@ -1836,12 +1887,14 @@
         <v>ecm4m-voc:atomprobetip</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>117</v>
+      </c>
       <c r="D35" s="3"/>
       <c r="E35" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F35" s="31"/>
       <c r="G35" s="31"/>
@@ -1861,12 +1914,14 @@
         <v>ecm4m-voc:microtomeslices</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C36" s="3"/>
+        <v>103</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="D36" s="3"/>
       <c r="E36" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F36" s="30"/>
       <c r="G36" s="30"/>
@@ -1886,12 +1941,14 @@
         <v>ecm4m-voc:residue</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="C37" s="4"/>
+        <v>104</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="D37" s="3"/>
       <c r="E37" s="29" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F37" s="31"/>
       <c r="G37" s="31"/>
@@ -1911,10 +1968,10 @@
         <v>ecm4m-voc:Non-PolishedSectionContainerType</v>
       </c>
       <c r="B38" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" s="25" t="s">
         <v>106</v>
-      </c>
-      <c r="C38" s="25" t="s">
-        <v>107</v>
       </c>
       <c r="D38" s="25"/>
       <c r="E38" s="27"/>
@@ -1938,12 +1995,12 @@
         <v>ecm4m-voc:aluminumcontainer</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C39" s="4"/>
       <c r="D39" s="3"/>
       <c r="E39" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F39" s="31"/>
       <c r="G39" s="31"/>
@@ -1963,12 +2020,12 @@
         <v>ecm4m-voc:glassvial</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
@@ -1988,12 +2045,12 @@
         <v>ecm4m-voc:teflonbag</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F41" s="31"/>
       <c r="G41" s="31"/>
@@ -2013,12 +2070,12 @@
         <v>ecm4m-voc:polycarbonatecontainer</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
@@ -2038,12 +2095,12 @@
         <v>ecm4m-voc:aluminumwrapping</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F43" s="31"/>
       <c r="G43" s="31"/>
@@ -2063,12 +2120,12 @@
         <v>ecm4m-voc:customcontainer</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="29" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
@@ -2084,14 +2141,14 @@
     </row>
     <row r="45" spans="1:16" ht="16">
       <c r="A45" s="24" t="str">
-        <f>IF(ISBLANK($B45),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B45," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" ref="A45:A51" si="4">IF(ISBLANK($B45),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B45," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
         <v>ecm4m-voc:PolishedSectionSampleType</v>
       </c>
       <c r="B45" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="C45" s="25" t="s">
         <v>88</v>
-      </c>
-      <c r="C45" s="25" t="s">
-        <v>89</v>
       </c>
       <c r="D45" s="25"/>
       <c r="E45" s="27"/>
@@ -2111,13 +2168,15 @@
     </row>
     <row r="46" spans="1:16" ht="16">
       <c r="A46" s="23" t="str">
-        <f>IF(ISBLANK($B46),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B46," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="4"/>
         <v>ecm4m-voc:thinSection</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="D46" s="4"/>
       <c r="E46" s="29" t="s">
         <v>113</v>
@@ -2136,13 +2195,15 @@
     </row>
     <row r="47" spans="1:16" ht="16">
       <c r="A47" s="23" t="str">
-        <f>IF(ISBLANK($B47),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B47," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="4"/>
         <v>ecm4m-voc:thickSection</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="C47" s="4"/>
+        <v>82</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>125</v>
+      </c>
       <c r="D47" s="4"/>
       <c r="E47" s="29" t="s">
         <v>113</v>
@@ -2161,13 +2222,15 @@
     </row>
     <row r="48" spans="1:16" ht="16">
       <c r="A48" s="23" t="str">
-        <f>IF(ISBLANK($B48),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B48," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="4"/>
         <v>ecm4m-voc:pottedButt</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="3"/>
+        <v>83</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>126</v>
+      </c>
       <c r="D48" s="3"/>
       <c r="E48" s="29" t="s">
         <v>113</v>
@@ -2186,13 +2249,15 @@
     </row>
     <row r="49" spans="1:16" ht="16">
       <c r="A49" s="23" t="str">
-        <f>IF(ISBLANK($B49),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B49," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="4"/>
         <v>ecm4m-voc:pressedGrainsEpoxy</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C49" s="3"/>
+        <v>84</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="D49" s="3"/>
       <c r="E49" s="29" t="s">
         <v>113</v>
@@ -2211,13 +2276,15 @@
     </row>
     <row r="50" spans="1:16" ht="16">
       <c r="A50" s="23" t="str">
-        <f>IF(ISBLANK($B50),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B50," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="4"/>
         <v>ecm4m-voc:pressedGrainsMetal</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C50" s="3"/>
+        <v>85</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="D50" s="3"/>
       <c r="E50" s="29" t="s">
         <v>113</v>
@@ -2236,14 +2303,14 @@
     </row>
     <row r="51" spans="1:16" ht="16">
       <c r="A51" s="24" t="str">
-        <f>IF(ISBLANK($B51),"",$B$3 &amp; ":" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B51," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <f t="shared" si="4"/>
         <v>ecm4m-voc:PolishedSectionContainerType</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" s="25"/>
       <c r="E51" s="27"/>
@@ -2267,12 +2334,12 @@
         <v>ecm4m-voc:ps_aluminumcontainer</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="3"/>
       <c r="E52" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="30"/>
@@ -2288,8 +2355,8 @@
     </row>
     <row r="53" spans="1:16" ht="16">
       <c r="A53" s="23" t="str">
-        <f t="shared" ref="A53:A57" si="4">IF(ISBLANK($B53),"",$B$3 &amp; ":ps_" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B53," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
-        <v>ecm4m-voc:ps_glassvial</v>
+        <f t="shared" ref="A53:A56" si="5">IF(ISBLANK($B53),"",$B$3 &amp; ":ps_" &amp; (SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(B53," ",""),"/","Div"),",","-"),"(","-"),")",""),"+","plus"),"--","-")," ",""),"&amp;","-")))</f>
+        <v>ecm4m-voc:ps_teflonbag</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>91</v>
@@ -2297,7 +2364,7 @@
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
       <c r="E53" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F53" s="30"/>
       <c r="G53" s="30"/>
@@ -2313,8 +2380,8 @@
     </row>
     <row r="54" spans="1:16" ht="16">
       <c r="A54" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>ecm4m-voc:ps_teflonbag</v>
+        <f t="shared" si="5"/>
+        <v>ecm4m-voc:ps_polycarbonatecontainer</v>
       </c>
       <c r="B54" s="3" t="s">
         <v>92</v>
@@ -2322,7 +2389,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
       <c r="E54" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F54" s="30"/>
       <c r="G54" s="30"/>
@@ -2338,8 +2405,8 @@
     </row>
     <row r="55" spans="1:16" ht="16">
       <c r="A55" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>ecm4m-voc:ps_polycarbonatecontainer</v>
+        <f t="shared" si="5"/>
+        <v>ecm4m-voc:ps_aluminumwrapping</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>93</v>
@@ -2347,7 +2414,7 @@
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F55" s="30"/>
       <c r="G55" s="30"/>
@@ -2363,8 +2430,8 @@
     </row>
     <row r="56" spans="1:16" ht="16">
       <c r="A56" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>ecm4m-voc:ps_aluminumwrapping</v>
+        <f t="shared" si="5"/>
+        <v>ecm4m-voc:ps_customcontainer</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>94</v>
@@ -2372,7 +2439,7 @@
       <c r="C56" s="3"/>
       <c r="D56" s="3"/>
       <c r="E56" s="29" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F56" s="30"/>
       <c r="G56" s="30"/>
@@ -2386,19 +2453,15 @@
       <c r="O56" s="45"/>
       <c r="P56" s="45"/>
     </row>
-    <row r="57" spans="1:16" ht="16">
+    <row r="57" spans="1:16" ht="15" customHeight="1">
       <c r="A57" s="23" t="str">
-        <f t="shared" si="4"/>
-        <v>ecm4m-voc:ps_customcontainer</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>95</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="B57" s="3"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3"/>
-      <c r="E57" s="29" t="s">
-        <v>114</v>
-      </c>
+      <c r="E57" s="29"/>
       <c r="F57" s="30"/>
       <c r="G57" s="30"/>
       <c r="H57" s="30"/>
@@ -2416,14 +2479,14 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="4"/>
       <c r="D58" s="3"/>
       <c r="E58" s="29"/>
-      <c r="F58" s="30"/>
-      <c r="G58" s="30"/>
-      <c r="H58" s="30"/>
-      <c r="I58" s="38"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
+      <c r="I58" s="40"/>
       <c r="J58" s="44"/>
       <c r="K58" s="46"/>
       <c r="L58" s="47"/>
@@ -2437,14 +2500,14 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
+      <c r="B59" s="3"/>
+      <c r="C59" s="3"/>
       <c r="D59" s="3"/>
       <c r="E59" s="29"/>
-      <c r="F59" s="31"/>
-      <c r="G59" s="31"/>
-      <c r="H59" s="31"/>
-      <c r="I59" s="40"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="30"/>
+      <c r="H59" s="30"/>
+      <c r="I59" s="38"/>
       <c r="J59" s="44"/>
       <c r="K59" s="46"/>
       <c r="L59" s="47"/>
@@ -2458,14 +2521,14 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="3"/>
+      <c r="B60" s="4"/>
+      <c r="C60" s="4"/>
       <c r="D60" s="3"/>
       <c r="E60" s="29"/>
-      <c r="F60" s="30"/>
-      <c r="G60" s="30"/>
-      <c r="H60" s="30"/>
-      <c r="I60" s="38"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31"/>
+      <c r="I60" s="40"/>
       <c r="J60" s="44"/>
       <c r="K60" s="46"/>
       <c r="L60" s="47"/>
@@ -2479,14 +2542,14 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
       <c r="D61" s="3"/>
       <c r="E61" s="29"/>
-      <c r="F61" s="31"/>
-      <c r="G61" s="31"/>
-      <c r="H61" s="31"/>
-      <c r="I61" s="40"/>
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="30"/>
+      <c r="I61" s="38"/>
       <c r="J61" s="44"/>
       <c r="K61" s="46"/>
       <c r="L61" s="47"/>
@@ -2500,14 +2563,14 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="B62" s="4"/>
+      <c r="C62" s="4"/>
       <c r="D62" s="3"/>
       <c r="E62" s="29"/>
-      <c r="F62" s="30"/>
-      <c r="G62" s="30"/>
-      <c r="H62" s="30"/>
-      <c r="I62" s="38"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
+      <c r="I62" s="40"/>
       <c r="J62" s="44"/>
       <c r="K62" s="46"/>
       <c r="L62" s="47"/>
@@ -2515,27 +2578,6 @@
       <c r="N62" s="45"/>
       <c r="O62" s="45"/>
       <c r="P62" s="45"/>
-    </row>
-    <row r="63" spans="1:16" ht="15" customHeight="1">
-      <c r="A63" s="23" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="29"/>
-      <c r="F63" s="31"/>
-      <c r="G63" s="31"/>
-      <c r="H63" s="31"/>
-      <c r="I63" s="40"/>
-      <c r="J63" s="44"/>
-      <c r="K63" s="46"/>
-      <c r="L63" s="47"/>
-      <c r="M63" s="47"/>
-      <c r="N63" s="45"/>
-      <c r="O63" s="45"/>
-      <c r="P63" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>